<commit_message>
Fix handle of format strings with strings or [colors] in them.
</commit_message>
<xml_diff>
--- a/test/files/formats.xlsx
+++ b/test/files/formats.xlsx
@@ -50,7 +50,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="62">
+  <numFmts count="74">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="166" formatCode="M/D/YY"/>
@@ -67,52 +67,64 @@
     <numFmt numFmtId="177" formatCode="[HH]:MM:SS"/>
     <numFmt numFmtId="178" formatCode="#,##0"/>
     <numFmt numFmtId="179" formatCode="MM/DD/YYYY"/>
-    <numFmt numFmtId="180" formatCode="MM:SS"/>
+    <numFmt numFmtId="180" formatCode="[HH]:MM:SS.00"/>
     <numFmt numFmtId="181" formatCode="#,##0.00"/>
     <numFmt numFmtId="182" formatCode="MMM\ D&quot;, &quot;YY"/>
-    <numFmt numFmtId="183" formatCode="[H]:MM:SS"/>
+    <numFmt numFmtId="183" formatCode="MM:SS"/>
     <numFmt numFmtId="184" formatCode="#,###.00"/>
     <numFmt numFmtId="185" formatCode="MMM\ D&quot;, &quot;YYYY"/>
-    <numFmt numFmtId="186" formatCode="#,##0_);\(#,##0\)"/>
-    <numFmt numFmtId="187" formatCode="D&quot;. &quot;MMM&quot;. &quot;YYYY"/>
-    <numFmt numFmtId="188" formatCode="#,##0.00_);\(#,##0.00\)"/>
-    <numFmt numFmtId="189" formatCode="MMMM\ D&quot;, &quot;YYYY"/>
-    <numFmt numFmtId="190" formatCode="0%"/>
-    <numFmt numFmtId="191" formatCode="D&quot;. &quot;MMMM\ YYYY"/>
-    <numFmt numFmtId="192" formatCode="0.00%"/>
-    <numFmt numFmtId="193" formatCode="DDD&quot;, &quot;MMM\ D&quot;, &quot;YY"/>
-    <numFmt numFmtId="194" formatCode="[$$-409]#,##0;\-[$$-409]#,##0"/>
-    <numFmt numFmtId="195" formatCode="DDD\ DD/MMM\ YY"/>
-    <numFmt numFmtId="196" formatCode="[$$-409]#,##0.00;\-[$$-409]#,##0.00"/>
-    <numFmt numFmtId="197" formatCode="DDD&quot;, &quot;MMMM\ D&quot;, &quot;YYYY"/>
-    <numFmt numFmtId="198" formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0"/>
-    <numFmt numFmtId="199" formatCode="DDDD&quot;, &quot;MMMM\ D&quot;, &quot;YYYY"/>
-    <numFmt numFmtId="200" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
-    <numFmt numFmtId="201" formatCode="MM\-DD"/>
-    <numFmt numFmtId="202" formatCode="[$$-409]#,##0.--;[RED]\-[$$-409]#,##0.--"/>
-    <numFmt numFmtId="203" formatCode="YY\-MM\-DD"/>
-    <numFmt numFmtId="204" formatCode="#,##0.00\ [$USD];\-#,##0.00\ [$USD]"/>
-    <numFmt numFmtId="205" formatCode="YYYY\-MM\-DD"/>
-    <numFmt numFmtId="206" formatCode="#,##0.00\ [$USD];[RED]\-#,##0.00\ [$USD]"/>
-    <numFmt numFmtId="207" formatCode="MM/YY"/>
-    <numFmt numFmtId="208" formatCode="[$$-409]* #,##0;\-[$$-409]* #,##0"/>
-    <numFmt numFmtId="209" formatCode="MMM\ DD"/>
-    <numFmt numFmtId="210" formatCode="[$$-409]* #,##0.00;\-[$$-409]* #,##0.00"/>
-    <numFmt numFmtId="211" formatCode="MMMM"/>
-    <numFmt numFmtId="212" formatCode="0.00E+000"/>
-    <numFmt numFmtId="213" formatCode="QQ\ YY"/>
-    <numFmt numFmtId="214" formatCode="0.00E+00"/>
-    <numFmt numFmtId="215" formatCode="WW"/>
-    <numFmt numFmtId="216" formatCode="##0.00E+00"/>
-    <numFmt numFmtId="217" formatCode="# ?/?"/>
-    <numFmt numFmtId="218" formatCode="# ??/??"/>
-    <numFmt numFmtId="219" formatCode="# ???/???"/>
-    <numFmt numFmtId="220" formatCode="# ?/2"/>
-    <numFmt numFmtId="221" formatCode="# ?/4"/>
-    <numFmt numFmtId="222" formatCode="# ?/8"/>
-    <numFmt numFmtId="223" formatCode="# ??/16"/>
-    <numFmt numFmtId="224" formatCode="# ??/10"/>
-    <numFmt numFmtId="225" formatCode="# ??/100"/>
+    <numFmt numFmtId="186" formatCode="[H]:MM:SS"/>
+    <numFmt numFmtId="187" formatCode="#,##0_);\(#,##0\)"/>
+    <numFmt numFmtId="188" formatCode="D&quot;. &quot;MMM&quot;. &quot;YYYY"/>
+    <numFmt numFmtId="189" formatCode="MM:SS.0"/>
+    <numFmt numFmtId="190" formatCode="#,##0.00_);\(#,##0.00\)"/>
+    <numFmt numFmtId="191" formatCode="MMMM\ D&quot;, &quot;YYYY"/>
+    <numFmt numFmtId="192" formatCode="0%"/>
+    <numFmt numFmtId="193" formatCode="D&quot;. &quot;MMMM\ YYYY"/>
+    <numFmt numFmtId="194" formatCode="0.00%"/>
+    <numFmt numFmtId="195" formatCode="DDD&quot;, &quot;MMM\ D&quot;, &quot;YY"/>
+    <numFmt numFmtId="196" formatCode="[$$-409]#,##0;\-[$$-409]#,##0"/>
+    <numFmt numFmtId="197" formatCode="DDD\ DD/MMM\ YY"/>
+    <numFmt numFmtId="198" formatCode="[$$-409]#,##0.00;\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="199" formatCode="DDD&quot;, &quot;MMMM\ D&quot;, &quot;YYYY"/>
+    <numFmt numFmtId="200" formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0"/>
+    <numFmt numFmtId="201" formatCode="DDDD&quot;, &quot;MMMM\ D&quot;, &quot;YYYY"/>
+    <numFmt numFmtId="202" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
+    <numFmt numFmtId="203" formatCode="MM\-DD"/>
+    <numFmt numFmtId="204" formatCode="[$$-409]#,##0.--;[RED]\-[$$-409]#,##0.--"/>
+    <numFmt numFmtId="205" formatCode="YY\-MM\-DD"/>
+    <numFmt numFmtId="206" formatCode="#,##0.00\ [$USD];\-#,##0.00\ [$USD]"/>
+    <numFmt numFmtId="207" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="208" formatCode="#,##0.00\ [$USD];[RED]\-#,##0.00\ [$USD]"/>
+    <numFmt numFmtId="209" formatCode="MM/YY"/>
+    <numFmt numFmtId="210" formatCode="[$$-409]* #,##0;\-[$$-409]* #,##0"/>
+    <numFmt numFmtId="211" formatCode="MMM\ DD"/>
+    <numFmt numFmtId="212" formatCode="[$$-409]* #,##0.00;\-[$$-409]* #,##0.00"/>
+    <numFmt numFmtId="213" formatCode="MMMM"/>
+    <numFmt numFmtId="214" formatCode="0.00E+000"/>
+    <numFmt numFmtId="215" formatCode="QQ\ YY"/>
+    <numFmt numFmtId="216" formatCode="0.00E+00"/>
+    <numFmt numFmtId="217" formatCode="WW"/>
+    <numFmt numFmtId="218" formatCode="##0.00E+00"/>
+    <numFmt numFmtId="219" formatCode="[$-1080409]DDDD&quot;, &quot;D\ MMMM\ YYYY"/>
+    <numFmt numFmtId="220" formatCode="# ?/?"/>
+    <numFmt numFmtId="221" formatCode="[$-1080409]DDDD&quot;, &quot;MMMM\ D\ YYYY"/>
+    <numFmt numFmtId="222" formatCode="# ??/??"/>
+    <numFmt numFmtId="223" formatCode="[$-1080409]DDD\ MMMM\ D\ YYYY"/>
+    <numFmt numFmtId="224" formatCode="# ???/???"/>
+    <numFmt numFmtId="225" formatCode="[$-1080409]DDD\ D\ MMMM\ YYYY"/>
+    <numFmt numFmtId="226" formatCode="# ?/2"/>
+    <numFmt numFmtId="227" formatCode="[$-1080409]D\ MMMM\ YYYY"/>
+    <numFmt numFmtId="228" formatCode="# ?/4"/>
+    <numFmt numFmtId="229" formatCode="[$-1080409]MMMM\ D\ YYYY"/>
+    <numFmt numFmtId="230" formatCode="# ?/8"/>
+    <numFmt numFmtId="231" formatCode="[$-1080409]D\ MMMM"/>
+    <numFmt numFmtId="232" formatCode="# ??/16"/>
+    <numFmt numFmtId="233" formatCode="[$-1080409]MMMM\ D"/>
+    <numFmt numFmtId="234" formatCode="# ??/10"/>
+    <numFmt numFmtId="235" formatCode="[$-1080409]MMMM\ YYYY"/>
+    <numFmt numFmtId="236" formatCode="# ??/100"/>
+    <numFmt numFmtId="237" formatCode="[$-1080409]MMMM"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -179,7 +191,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="74">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -425,6 +437,54 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="225" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="226" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="227" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="228" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="229" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="230" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="231" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="232" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="233" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="234" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="235" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="236" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="237" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -448,7 +508,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -582,26 +642,32 @@
       <c r="C7" s="21" t="n">
         <v>-12345.678900463</v>
       </c>
+      <c r="F7" s="22" t="n">
+        <v>-0.321099537037037</v>
+      </c>
       <c r="G7" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="22" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C8" s="23" t="n">
-        <v>-12345.678900463</v>
+      <c r="B8" s="23" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C8" s="24" t="n">
+        <v>-12345.678900463</v>
+      </c>
+      <c r="F8" s="25" t="n">
+        <v>-0.321099537037037</v>
       </c>
       <c r="G8" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="24" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C9" s="25" t="n">
+      <c r="B9" s="26" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C9" s="27" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G9" s="0" t="s">
@@ -609,10 +675,10 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="26" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C10" s="27" t="n">
+      <c r="B10" s="28" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C10" s="29" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G10" s="0" t="s">
@@ -620,10 +686,10 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="28" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C11" s="29" t="n">
+      <c r="B11" s="30" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C11" s="31" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G11" s="0" t="s">
@@ -631,10 +697,10 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="30" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C12" s="31" t="n">
+      <c r="B12" s="32" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C12" s="33" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G12" s="0" t="s">
@@ -642,10 +708,10 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="32" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C13" s="33" t="n">
+      <c r="B13" s="34" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C13" s="35" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G13" s="0" t="s">
@@ -653,10 +719,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="34" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C14" s="35" t="n">
+      <c r="B14" s="36" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C14" s="37" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G14" s="0" t="s">
@@ -664,10 +730,10 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="36" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C15" s="37" t="n">
+      <c r="B15" s="38" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C15" s="39" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G15" s="0" t="s">
@@ -675,10 +741,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="38" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C16" s="39" t="n">
+      <c r="B16" s="40" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C16" s="41" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G16" s="0" t="s">
@@ -686,10 +752,10 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="40" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C17" s="41" t="n">
+      <c r="B17" s="42" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C17" s="43" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G17" s="0" t="s">
@@ -697,10 +763,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="42" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C18" s="43" t="n">
+      <c r="B18" s="44" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C18" s="45" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G18" s="0" t="s">
@@ -708,10 +774,10 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="44" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C19" s="45" t="n">
+      <c r="B19" s="46" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C19" s="47" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G19" s="0" t="s">
@@ -719,10 +785,10 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="46" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C20" s="47" t="n">
+      <c r="B20" s="48" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C20" s="49" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G20" s="0" t="s">
@@ -730,10 +796,10 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="48" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C21" s="49" t="n">
+      <c r="B21" s="50" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C21" s="51" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G21" s="0" t="s">
@@ -741,10 +807,10 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="50" t="n">
-        <v>-12345.6789</v>
-      </c>
-      <c r="C22" s="51" t="n">
+      <c r="B22" s="52" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C22" s="53" t="n">
         <v>-12345.678900463</v>
       </c>
       <c r="G22" s="0" t="s">
@@ -752,80 +818,110 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="52" t="n">
-        <v>-12345.6789</v>
+      <c r="B23" s="54" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C23" s="55" t="n">
+        <v>-12345.678900463</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="53" t="n">
-        <v>-12345.6789</v>
+      <c r="B24" s="56" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C24" s="57" t="n">
+        <v>-12345.678900463</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="54" t="n">
-        <v>-12345.6789</v>
+      <c r="B25" s="58" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C25" s="59" t="n">
+        <v>-12345.678900463</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="55" t="n">
-        <v>-12345.6789</v>
+      <c r="B26" s="60" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C26" s="61" t="n">
+        <v>-12345.678900463</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="56" t="n">
-        <v>-12345.6789</v>
+      <c r="B27" s="62" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C27" s="63" t="n">
+        <v>-12345.678900463</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="57" t="n">
-        <v>-12345.6789</v>
+      <c r="B28" s="64" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C28" s="65" t="n">
+        <v>-12345.678900463</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="58" t="n">
-        <v>-12345.6789</v>
+      <c r="B29" s="66" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C29" s="67" t="n">
+        <v>-12345.678900463</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="59" t="n">
-        <v>-12345.6789</v>
+      <c r="B30" s="68" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C30" s="69" t="n">
+        <v>-12345.678900463</v>
       </c>
       <c r="G30" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="60" t="n">
-        <v>-12345.6789</v>
+      <c r="B31" s="70" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C31" s="71" t="n">
+        <v>-12345.678900463</v>
       </c>
       <c r="G31" s="0" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="61" t="n">
-        <v>-12345.6789</v>
+      <c r="B32" s="72" t="n">
+        <v>-12345.6789</v>
+      </c>
+      <c r="C32" s="73" t="n">
+        <v>-12345.678900463</v>
       </c>
       <c r="G32" s="0" t="s">
         <v>7</v>

</xml_diff>